<commit_message>
Add ExposureGroup <-> Portname config file mapping and use that for 3b vs 3d comparisons
</commit_message>
<xml_diff>
--- a/workspace/tests/files/invalid_config_broken_fk_import_file.xlsx
+++ b/workspace/tests/files/invalid_config_broken_fk_import_file.xlsx
@@ -17,6 +17,7 @@
     <sheet name="Groupings" sheetId="8" state="visible" r:id="rId8"/>
     <sheet name="Products and Perils" sheetId="9" state="visible" r:id="rId9"/>
     <sheet name="Moody's Reference Data" sheetId="10" state="visible" r:id="rId10"/>
+    <sheet name="ExposureGroup &lt;-&gt; Portname" sheetId="11" state="visible" r:id="rId11"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -425,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1500,6 +1501,121 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>ExposureGroup</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Portname</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>USHU_Hurricane_Full</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>USHU</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>USEQ</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>USEQ</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>USFL_Flood_Full</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>USFL</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>CBHU_Hurricane_Full</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>CBHU</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>CBEQ_QuakeBC</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>CBEQ</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>MEHU</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>MEHU</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>PRHU</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>PRHU</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
@@ -5899,7 +6015,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P499"/>
+  <dimension ref="A1:P94"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -10100,411 +10216,6 @@
         </is>
       </c>
     </row>
-    <row r="95"/>
-    <row r="96"/>
-    <row r="97"/>
-    <row r="98"/>
-    <row r="99"/>
-    <row r="100"/>
-    <row r="101"/>
-    <row r="102"/>
-    <row r="103"/>
-    <row r="104"/>
-    <row r="105"/>
-    <row r="106"/>
-    <row r="107"/>
-    <row r="108"/>
-    <row r="109"/>
-    <row r="110"/>
-    <row r="111"/>
-    <row r="112"/>
-    <row r="113"/>
-    <row r="114"/>
-    <row r="115"/>
-    <row r="116"/>
-    <row r="117"/>
-    <row r="118"/>
-    <row r="119"/>
-    <row r="120"/>
-    <row r="121"/>
-    <row r="122"/>
-    <row r="123"/>
-    <row r="124"/>
-    <row r="125"/>
-    <row r="126"/>
-    <row r="127"/>
-    <row r="128"/>
-    <row r="129"/>
-    <row r="130"/>
-    <row r="131"/>
-    <row r="132"/>
-    <row r="133"/>
-    <row r="134"/>
-    <row r="135"/>
-    <row r="136"/>
-    <row r="137"/>
-    <row r="138"/>
-    <row r="139"/>
-    <row r="140"/>
-    <row r="141"/>
-    <row r="142"/>
-    <row r="143"/>
-    <row r="144"/>
-    <row r="145"/>
-    <row r="146"/>
-    <row r="147"/>
-    <row r="148"/>
-    <row r="149"/>
-    <row r="150"/>
-    <row r="151"/>
-    <row r="152"/>
-    <row r="153"/>
-    <row r="154"/>
-    <row r="155"/>
-    <row r="156"/>
-    <row r="157"/>
-    <row r="158"/>
-    <row r="159"/>
-    <row r="160"/>
-    <row r="161"/>
-    <row r="162"/>
-    <row r="163"/>
-    <row r="164"/>
-    <row r="165"/>
-    <row r="166"/>
-    <row r="167"/>
-    <row r="168"/>
-    <row r="169"/>
-    <row r="170"/>
-    <row r="171"/>
-    <row r="172"/>
-    <row r="173"/>
-    <row r="174"/>
-    <row r="175"/>
-    <row r="176"/>
-    <row r="177"/>
-    <row r="178"/>
-    <row r="179"/>
-    <row r="180"/>
-    <row r="181"/>
-    <row r="182"/>
-    <row r="183"/>
-    <row r="184"/>
-    <row r="185"/>
-    <row r="186"/>
-    <row r="187"/>
-    <row r="188"/>
-    <row r="189"/>
-    <row r="190"/>
-    <row r="191"/>
-    <row r="192"/>
-    <row r="193"/>
-    <row r="194"/>
-    <row r="195"/>
-    <row r="196"/>
-    <row r="197"/>
-    <row r="198"/>
-    <row r="199"/>
-    <row r="200"/>
-    <row r="201"/>
-    <row r="202"/>
-    <row r="203"/>
-    <row r="204"/>
-    <row r="205"/>
-    <row r="206"/>
-    <row r="207"/>
-    <row r="208"/>
-    <row r="209"/>
-    <row r="210"/>
-    <row r="211"/>
-    <row r="212"/>
-    <row r="213"/>
-    <row r="214"/>
-    <row r="215"/>
-    <row r="216"/>
-    <row r="217"/>
-    <row r="218"/>
-    <row r="219"/>
-    <row r="220"/>
-    <row r="221"/>
-    <row r="222"/>
-    <row r="223"/>
-    <row r="224"/>
-    <row r="225"/>
-    <row r="226"/>
-    <row r="227"/>
-    <row r="228"/>
-    <row r="229"/>
-    <row r="230"/>
-    <row r="231"/>
-    <row r="232"/>
-    <row r="233"/>
-    <row r="234"/>
-    <row r="235"/>
-    <row r="236"/>
-    <row r="237"/>
-    <row r="238"/>
-    <row r="239"/>
-    <row r="240"/>
-    <row r="241"/>
-    <row r="242"/>
-    <row r="243"/>
-    <row r="244"/>
-    <row r="245"/>
-    <row r="246"/>
-    <row r="247"/>
-    <row r="248"/>
-    <row r="249"/>
-    <row r="250"/>
-    <row r="251"/>
-    <row r="252"/>
-    <row r="253"/>
-    <row r="254"/>
-    <row r="255"/>
-    <row r="256"/>
-    <row r="257"/>
-    <row r="258"/>
-    <row r="259"/>
-    <row r="260"/>
-    <row r="261"/>
-    <row r="262"/>
-    <row r="263"/>
-    <row r="264"/>
-    <row r="265"/>
-    <row r="266"/>
-    <row r="267"/>
-    <row r="268"/>
-    <row r="269"/>
-    <row r="270"/>
-    <row r="271"/>
-    <row r="272"/>
-    <row r="273"/>
-    <row r="274"/>
-    <row r="275"/>
-    <row r="276"/>
-    <row r="277"/>
-    <row r="278"/>
-    <row r="279"/>
-    <row r="280"/>
-    <row r="281"/>
-    <row r="282"/>
-    <row r="283"/>
-    <row r="284"/>
-    <row r="285"/>
-    <row r="286"/>
-    <row r="287"/>
-    <row r="288"/>
-    <row r="289"/>
-    <row r="290"/>
-    <row r="291"/>
-    <row r="292"/>
-    <row r="293"/>
-    <row r="294"/>
-    <row r="295"/>
-    <row r="296"/>
-    <row r="297"/>
-    <row r="298"/>
-    <row r="299"/>
-    <row r="300"/>
-    <row r="301"/>
-    <row r="302"/>
-    <row r="303"/>
-    <row r="304"/>
-    <row r="305"/>
-    <row r="306"/>
-    <row r="307"/>
-    <row r="308"/>
-    <row r="309"/>
-    <row r="310"/>
-    <row r="311"/>
-    <row r="312"/>
-    <row r="313"/>
-    <row r="314"/>
-    <row r="315"/>
-    <row r="316"/>
-    <row r="317"/>
-    <row r="318"/>
-    <row r="319"/>
-    <row r="320"/>
-    <row r="321"/>
-    <row r="322"/>
-    <row r="323"/>
-    <row r="324"/>
-    <row r="325"/>
-    <row r="326"/>
-    <row r="327"/>
-    <row r="328"/>
-    <row r="329"/>
-    <row r="330"/>
-    <row r="331"/>
-    <row r="332"/>
-    <row r="333"/>
-    <row r="334"/>
-    <row r="335"/>
-    <row r="336"/>
-    <row r="337"/>
-    <row r="338"/>
-    <row r="339"/>
-    <row r="340"/>
-    <row r="341"/>
-    <row r="342"/>
-    <row r="343"/>
-    <row r="344"/>
-    <row r="345"/>
-    <row r="346"/>
-    <row r="347"/>
-    <row r="348"/>
-    <row r="349"/>
-    <row r="350"/>
-    <row r="351"/>
-    <row r="352"/>
-    <row r="353"/>
-    <row r="354"/>
-    <row r="355"/>
-    <row r="356"/>
-    <row r="357"/>
-    <row r="358"/>
-    <row r="359"/>
-    <row r="360"/>
-    <row r="361"/>
-    <row r="362"/>
-    <row r="363"/>
-    <row r="364"/>
-    <row r="365"/>
-    <row r="366"/>
-    <row r="367"/>
-    <row r="368"/>
-    <row r="369"/>
-    <row r="370"/>
-    <row r="371"/>
-    <row r="372"/>
-    <row r="373"/>
-    <row r="374"/>
-    <row r="375"/>
-    <row r="376"/>
-    <row r="377"/>
-    <row r="378"/>
-    <row r="379"/>
-    <row r="380"/>
-    <row r="381"/>
-    <row r="382"/>
-    <row r="383"/>
-    <row r="384"/>
-    <row r="385"/>
-    <row r="386"/>
-    <row r="387"/>
-    <row r="388"/>
-    <row r="389"/>
-    <row r="390"/>
-    <row r="391"/>
-    <row r="392"/>
-    <row r="393"/>
-    <row r="394"/>
-    <row r="395"/>
-    <row r="396"/>
-    <row r="397"/>
-    <row r="398"/>
-    <row r="399"/>
-    <row r="400"/>
-    <row r="401"/>
-    <row r="402"/>
-    <row r="403"/>
-    <row r="404"/>
-    <row r="405"/>
-    <row r="406"/>
-    <row r="407"/>
-    <row r="408"/>
-    <row r="409"/>
-    <row r="410"/>
-    <row r="411"/>
-    <row r="412"/>
-    <row r="413"/>
-    <row r="414"/>
-    <row r="415"/>
-    <row r="416"/>
-    <row r="417"/>
-    <row r="418"/>
-    <row r="419"/>
-    <row r="420"/>
-    <row r="421"/>
-    <row r="422"/>
-    <row r="423"/>
-    <row r="424"/>
-    <row r="425"/>
-    <row r="426"/>
-    <row r="427"/>
-    <row r="428"/>
-    <row r="429"/>
-    <row r="430"/>
-    <row r="431"/>
-    <row r="432"/>
-    <row r="433"/>
-    <row r="434"/>
-    <row r="435"/>
-    <row r="436"/>
-    <row r="437"/>
-    <row r="438"/>
-    <row r="439"/>
-    <row r="440"/>
-    <row r="441"/>
-    <row r="442"/>
-    <row r="443"/>
-    <row r="444"/>
-    <row r="445"/>
-    <row r="446"/>
-    <row r="447"/>
-    <row r="448"/>
-    <row r="449"/>
-    <row r="450"/>
-    <row r="451"/>
-    <row r="452"/>
-    <row r="453"/>
-    <row r="454"/>
-    <row r="455"/>
-    <row r="456"/>
-    <row r="457"/>
-    <row r="458"/>
-    <row r="459"/>
-    <row r="460"/>
-    <row r="461"/>
-    <row r="462"/>
-    <row r="463"/>
-    <row r="464"/>
-    <row r="465"/>
-    <row r="466"/>
-    <row r="467"/>
-    <row r="468"/>
-    <row r="469"/>
-    <row r="470"/>
-    <row r="471"/>
-    <row r="472"/>
-    <row r="473"/>
-    <row r="474"/>
-    <row r="475"/>
-    <row r="476"/>
-    <row r="477"/>
-    <row r="478"/>
-    <row r="479"/>
-    <row r="480"/>
-    <row r="481"/>
-    <row r="482"/>
-    <row r="483"/>
-    <row r="484"/>
-    <row r="485"/>
-    <row r="486"/>
-    <row r="487"/>
-    <row r="488"/>
-    <row r="489"/>
-    <row r="490"/>
-    <row r="491"/>
-    <row r="492"/>
-    <row r="493"/>
-    <row r="494"/>
-    <row r="495"/>
-    <row r="496"/>
-    <row r="497"/>
-    <row r="498"/>
-    <row r="499"/>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>